<commit_message>
lab corrigé, voir commentaires dans doc xls
</commit_message>
<xml_diff>
--- a/Projet- Mouad1/LabsGrilleDeCorrection.xlsx
+++ b/Projet- Mouad1/LabsGrilleDeCorrection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab2 - Globex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab2 - Globex/Groupe4/Lab2-GlobeX-Groupe4/Projet- Mouad1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{7AB2CD5E-D875-4634-96BE-3587703DCB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E104E26-3222-4CCF-8857-CB73E9047493}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{7AB2CD5E-D875-4634-96BE-3587703DCB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69D04CBD-5F5A-4346-8D75-851A2497A4ED}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E104A93-42AC-4B01-B277-A83AFE77E344}"/>
+    <workbookView xWindow="-55650" yWindow="9435" windowWidth="17595" windowHeight="19320" xr2:uid="{6E104A93-42AC-4B01-B277-A83AFE77E344}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Exigences</t>
   </si>
@@ -93,6 +93,27 @@
   </si>
   <si>
     <t>Commentaires</t>
+  </si>
+  <si>
+    <t>*****mauve sur noir n'est pas lisible</t>
+  </si>
+  <si>
+    <t>* ID's sont unique et ne peuvent pas être utiliser plus qu'une fois dans le document</t>
+  </si>
+  <si>
+    <t>voir commentaire de navigation</t>
+  </si>
+  <si>
+    <t>confusion sur quel document à coriger, vue que deux fichier de projets on été remis</t>
+  </si>
+  <si>
+    <t>description n'as pas été modifier de stock</t>
+  </si>
+  <si>
+    <t>aucun commentaires</t>
+  </si>
+  <si>
+    <t>erreurs dans le CSS ** balises &lt;style&gt; ne vont pas dans un fichier .css</t>
   </si>
 </sst>
 </file>
@@ -450,7 +471,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +501,10 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -488,6 +513,10 @@
       <c r="B3">
         <v>8</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -496,6 +525,10 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -504,6 +537,10 @@
       <c r="B5">
         <v>10</v>
       </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -512,6 +549,12 @@
       <c r="B6">
         <v>10</v>
       </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -520,6 +563,12 @@
       <c r="B7">
         <v>10</v>
       </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -528,6 +577,10 @@
       <c r="B8">
         <v>10</v>
       </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -536,6 +589,12 @@
       <c r="B9">
         <v>10</v>
       </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -544,13 +603,25 @@
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11">
         <v>10</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -560,6 +631,12 @@
       <c r="B12">
         <v>10</v>
       </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -568,6 +645,12 @@
       <c r="B13">
         <v>10</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -576,6 +659,10 @@
       <c r="B14">
         <v>5</v>
       </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -587,8 +674,9 @@
       </c>
       <c r="C15">
         <f>SUM(C2:C14)</f>
-        <v>0</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -596,7 +684,7 @@
       </c>
       <c r="C16">
         <f>C15/B15*100</f>
-        <v>0</v>
+        <v>72.916666666666657</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>